<commit_message>
Se añadió la conexión a S3 de codigo Red
</commit_message>
<xml_diff>
--- a/out/Armónicas en Corrientes/tablas/tdd_porcentaje.xlsx
+++ b/out/Armónicas en Corrientes/tablas/tdd_porcentaje.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae599aac914ac79b/Desktop/VSCodeProyectos/Python/MVP_InnovaPQ/out/Armónicas en Corrientes/tablas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_1C5DE13124D19E53309A6312E58EDB0236E0510A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -40,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +110,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,7 +162,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -182,6 +196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -391,14 +407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,24 +437,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3.848</v>
+        <v>3.8479999999999999</v>
       </c>
       <c r="B2">
-        <v>4.88945</v>
+        <v>4.8894500000000001</v>
       </c>
       <c r="C2">
-        <v>6.074166666666667</v>
+        <v>6.0741666666666667</v>
       </c>
       <c r="D2">
-        <v>6.163215277777778</v>
+        <v>6.1632152777777778</v>
       </c>
       <c r="E2">
-        <v>7.857949999999996</v>
+        <v>7.8579499999999962</v>
       </c>
       <c r="F2">
-        <v>8.67474</v>
+        <v>8.6747399999999999</v>
       </c>
       <c r="G2">
         <v>9.952</v>

</xml_diff>